<commit_message>
add search for all modules
</commit_message>
<xml_diff>
--- a/main/static/records/poc_contacts.xlsx
+++ b/main/static/records/poc_contacts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,39 +20,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
   <si>
-    <t xml:space="preserve">+639159484200</t>
+    <t xml:space="preserve">09176214704</t>
   </si>
   <si>
-    <t xml:space="preserve">ABAC, AILYN-AGN</t>
+    <t xml:space="preserve">Jasper Barcelona</t>
   </si>
   <si>
-    <t xml:space="preserve">AGN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09189123948</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABAD, LANDELINA ORCIGA-ANB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ANB</t>
+    <t xml:space="preserve">New Group</t>
   </si>
   <si>
     <t xml:space="preserve">09772312533</t>
   </si>
   <si>
-    <t xml:space="preserve">ABAD, NELSON M.-JNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">JNC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09162771025</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BABAD, NELSON M.-JNC</t>
+    <t xml:space="preserve">Leanza Etorma</t>
   </si>
 </sst>
 </file>
@@ -68,6 +50,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -153,17 +136,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.8877551020408"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="31.2551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -185,29 +168,7 @@
         <v>4</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug in change password
</commit_message>
<xml_diff>
--- a/main/static/records/poc_contacts.xlsx
+++ b/main/static/records/poc_contacts.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,21 +20,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">09176214704</t>
   </si>
   <si>
-    <t xml:space="preserve">Jasper Barcelona</t>
+    <t xml:space="preserve">Leanza Etorma</t>
   </si>
   <si>
-    <t xml:space="preserve">New Group</t>
-  </si>
-  <si>
-    <t xml:space="preserve">09772312533</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leanza Etorma</t>
+    <t xml:space="preserve">Sample Group</t>
   </si>
 </sst>
 </file>
@@ -136,17 +130,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="17.5510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -160,17 +155,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>2</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>